<commit_message>
update FT, prestart et rapport us
</commit_message>
<xml_diff>
--- a/lib/PHPExcel/templates/FT.xlsx
+++ b/lib/PHPExcel/templates/FT.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="151">
   <si>
     <t>MACHINING</t>
   </si>
@@ -198,9 +198,6 @@
   </si>
   <si>
     <t>Prefixe</t>
-  </si>
-  <si>
-    <t>Chk</t>
   </si>
   <si>
     <t>Date</t>
@@ -647,11 +644,73 @@
   <si>
     <t>---Quels commentaires afficher ? Instruction/commentaire job, split, eprouvettes ?</t>
   </si>
+  <si>
+    <t>affichage delai ?</t>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF8E98A5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8E98A5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Check</t>
+    </r>
+  </si>
+  <si>
+    <t>Grey cell : unused equipement or information (unless specified) -- Instructions on GPM need to be checked if checker is empty</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF8E98A5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Specimen) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF8E98A5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Checker</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF8E98A5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (Test)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="33">
     <font>
       <sz val="10"/>
@@ -849,7 +908,7 @@
       <charset val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -865,14 +924,8 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1057,11 +1110,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1213,7 +1275,6 @@
     <xf numFmtId="0" fontId="22" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1237,9 +1298,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1318,6 +1376,9 @@
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
@@ -1330,13 +1391,12 @@
     <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
@@ -1344,6 +1404,23 @@
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1814,10 +1891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R52"/>
+  <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
@@ -1843,12 +1920,12 @@
       <c r="L2" s="22"/>
       <c r="M2" s="22"/>
       <c r="N2" s="18"/>
-      <c r="O2" s="66" t="s">
-        <v>40</v>
+      <c r="O2" s="106" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="18" customHeight="1">
-      <c r="O3" s="66"/>
+      <c r="O3" s="106"/>
     </row>
     <row r="4" spans="1:18" ht="18" customHeight="1">
       <c r="A4" s="28" t="s">
@@ -1860,29 +1937,29 @@
       </c>
       <c r="E4" s="27"/>
       <c r="G4" s="29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H4" s="28"/>
       <c r="I4" s="2"/>
       <c r="J4" s="29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K4" s="28"/>
       <c r="L4" s="2"/>
       <c r="M4" s="29"/>
-      <c r="N4" s="92" t="s">
-        <v>82</v>
-      </c>
-      <c r="O4" s="66"/>
+      <c r="N4" s="90" t="s">
+        <v>81</v>
+      </c>
+      <c r="O4" s="106"/>
     </row>
     <row r="5" spans="1:18" ht="18.95" customHeight="1">
       <c r="A5" s="49" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="49"/>
       <c r="C5" s="50"/>
       <c r="D5" s="49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="49"/>
       <c r="F5" s="50"/>
@@ -1900,32 +1977,32 @@
         <v>5</v>
       </c>
       <c r="N5" s="49"/>
-      <c r="O5" s="66"/>
+      <c r="O5" s="106"/>
     </row>
     <row r="6" spans="1:18" ht="18.95" customHeight="1">
       <c r="A6" s="29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="28"/>
       <c r="D6" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E6" s="28"/>
       <c r="G6" s="29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H6" s="30"/>
-      <c r="I6" s="4"/>
+      <c r="I6" s="92"/>
       <c r="J6" s="29" t="s">
-        <v>81</v>
+        <v>150</v>
       </c>
       <c r="K6" s="30"/>
-      <c r="L6" s="4"/>
+      <c r="L6" s="103"/>
       <c r="M6" s="30"/>
-      <c r="N6" s="93" t="s">
-        <v>144</v>
-      </c>
-      <c r="O6" s="66"/>
+      <c r="N6" s="91" t="s">
+        <v>143</v>
+      </c>
+      <c r="O6" s="106"/>
     </row>
     <row r="7" spans="1:18" ht="18.95" customHeight="1">
       <c r="A7" s="49">
@@ -1934,17 +2011,17 @@
       <c r="B7" s="49"/>
       <c r="C7" s="50"/>
       <c r="D7" s="49" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E7" s="49"/>
       <c r="F7" s="50"/>
       <c r="G7" s="49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H7" s="49"/>
       <c r="I7" s="51"/>
       <c r="J7" s="49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K7" s="49"/>
       <c r="L7" s="51"/>
@@ -1952,12 +2029,12 @@
         <v>5</v>
       </c>
       <c r="N7" s="49"/>
-      <c r="O7" s="66"/>
+      <c r="O7" s="106"/>
     </row>
     <row r="8" spans="1:18" ht="6" customHeight="1"/>
     <row r="9" spans="1:18" ht="15" customHeight="1">
       <c r="A9" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
@@ -1978,53 +2055,53 @@
     <row r="10" spans="1:18" ht="5.25" customHeight="1"/>
     <row r="11" spans="1:18" s="38" customFormat="1">
       <c r="A11" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11" s="34"/>
       <c r="C11" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D11" s="34"/>
       <c r="E11" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H11" s="34"/>
       <c r="I11" s="35"/>
       <c r="J11" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="K11" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="K11" s="36" t="s">
-        <v>84</v>
-      </c>
       <c r="L11" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="M11" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="M11" s="36" t="s">
+      <c r="N11" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="N11" s="36" t="s">
-        <v>48</v>
-      </c>
       <c r="O11" s="36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P11" s="37" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q11" s="25"/>
       <c r="R11" s="25"/>
     </row>
     <row r="12" spans="1:18" ht="14.25">
       <c r="A12" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B12" s="31"/>
       <c r="C12" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D12" s="31"/>
       <c r="E12" s="31">
@@ -2032,71 +2109,71 @@
       </c>
       <c r="F12" s="31"/>
       <c r="G12" s="44" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H12" s="31"/>
       <c r="I12" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="J12" s="62" t="s">
-        <v>119</v>
-      </c>
-      <c r="K12" s="62">
+        <v>48</v>
+      </c>
+      <c r="J12" s="61" t="s">
+        <v>118</v>
+      </c>
+      <c r="K12" s="61">
         <v>80</v>
       </c>
-      <c r="L12" s="62" t="s">
-        <v>73</v>
-      </c>
-      <c r="M12" s="62" t="s">
-        <v>73</v>
-      </c>
-      <c r="N12" s="62" t="s">
-        <v>73</v>
-      </c>
-      <c r="O12" s="62" t="s">
-        <v>73</v>
-      </c>
-      <c r="P12" s="63" t="s">
-        <v>73</v>
+      <c r="L12" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="M12" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="N12" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="O12" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="P12" s="62" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:18" s="38" customFormat="1">
       <c r="A13" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" s="34"/>
       <c r="C13" s="34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D13" s="34"/>
       <c r="E13" s="34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F13" s="34"/>
       <c r="G13" s="34"/>
       <c r="H13" s="34"/>
       <c r="I13" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="J13" s="62" t="s">
-        <v>120</v>
-      </c>
-      <c r="K13" s="62">
+        <v>50</v>
+      </c>
+      <c r="J13" s="61" t="s">
+        <v>119</v>
+      </c>
+      <c r="K13" s="61">
         <v>100</v>
       </c>
-      <c r="L13" s="62">
+      <c r="L13" s="61">
         <v>3</v>
       </c>
-      <c r="M13" s="62">
+      <c r="M13" s="61">
         <v>0.3</v>
       </c>
-      <c r="N13" s="62">
+      <c r="N13" s="61">
         <v>0</v>
       </c>
-      <c r="O13" s="62">
+      <c r="O13" s="61">
         <v>10</v>
       </c>
-      <c r="P13" s="63">
+      <c r="P13" s="62">
         <v>1</v>
       </c>
       <c r="Q13" s="25"/>
@@ -2112,33 +2189,33 @@
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F14" s="31"/>
       <c r="G14" s="31"/>
       <c r="H14" s="31"/>
       <c r="I14" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="J14" s="64">
+        <v>51</v>
+      </c>
+      <c r="J14" s="63">
         <v>10005</v>
       </c>
-      <c r="K14" s="64">
+      <c r="K14" s="63">
         <v>5</v>
       </c>
-      <c r="L14" s="64">
+      <c r="L14" s="63">
         <v>1500</v>
       </c>
-      <c r="M14" s="64">
+      <c r="M14" s="63">
         <v>150</v>
       </c>
-      <c r="N14" s="64">
+      <c r="N14" s="63">
         <v>0</v>
       </c>
-      <c r="O14" s="64">
+      <c r="O14" s="63">
         <v>40</v>
       </c>
-      <c r="P14" s="65">
+      <c r="P14" s="64">
         <v>0.5</v>
       </c>
     </row>
@@ -2147,7 +2224,7 @@
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1">
       <c r="A16" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
@@ -2173,7 +2250,7 @@
     </row>
     <row r="18" spans="1:18" ht="12.75" customHeight="1">
       <c r="E18" s="34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="34"/>
@@ -2181,7 +2258,7 @@
       <c r="I18" s="34"/>
       <c r="J18" s="34"/>
       <c r="K18" s="34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L18" s="34"/>
       <c r="M18" s="34"/>
@@ -2193,31 +2270,31 @@
       </c>
       <c r="B19" s="34"/>
       <c r="C19" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D19" s="34"/>
       <c r="E19" s="34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H19" s="34"/>
       <c r="I19" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J19" s="34"/>
       <c r="K19" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L19" s="34"/>
       <c r="M19" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N19" s="34"/>
       <c r="O19" s="34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P19" s="34"/>
       <c r="Q19" s="25"/>
@@ -2225,23 +2302,23 @@
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B20" s="49"/>
       <c r="C20" s="49" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D20" s="49"/>
-      <c r="E20" s="49">
+      <c r="E20" s="107">
         <v>4.37</v>
       </c>
       <c r="F20" s="49"/>
       <c r="G20" s="49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H20" s="49"/>
       <c r="I20" s="49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J20" s="49"/>
       <c r="K20" s="49">
@@ -2259,49 +2336,49 @@
     </row>
     <row r="21" spans="1:18" s="38" customFormat="1">
       <c r="A21" s="34"/>
-      <c r="B21" s="81" t="s">
+      <c r="B21" s="79" t="s">
+        <v>130</v>
+      </c>
+      <c r="C21" s="34" t="s">
         <v>131</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>132</v>
       </c>
       <c r="D21" s="34"/>
       <c r="E21" s="34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H21" s="34"/>
-      <c r="I21" s="82"/>
+      <c r="I21" s="80"/>
       <c r="J21" s="41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K21" s="34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L21" s="34"/>
       <c r="M21" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N21" s="34"/>
       <c r="O21" s="34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P21" s="34"/>
       <c r="Q21" s="25"/>
       <c r="R21" s="25"/>
     </row>
     <row r="22" spans="1:18">
-      <c r="A22" s="80" t="s">
-        <v>129</v>
-      </c>
-      <c r="B22" s="94">
+      <c r="A22" s="105" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" s="93">
         <v>180</v>
       </c>
       <c r="C22" s="49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D22" s="49"/>
       <c r="E22" s="31">
@@ -2309,14 +2386,14 @@
       </c>
       <c r="F22" s="31"/>
       <c r="G22" s="31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H22" s="31"/>
       <c r="I22" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J22" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K22" s="49">
         <v>0.6</v>
@@ -2332,36 +2409,36 @@
       <c r="P22" s="49"/>
     </row>
     <row r="23" spans="1:18" ht="15.75">
-      <c r="A23" s="80" t="s">
-        <v>130</v>
-      </c>
-      <c r="B23" s="95">
+      <c r="A23" s="78" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" s="94">
         <v>170</v>
       </c>
       <c r="C23" s="52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D23" s="52"/>
       <c r="E23" s="46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F23" s="46"/>
       <c r="G23" s="47"/>
       <c r="H23" s="46"/>
       <c r="I23" s="47"/>
       <c r="J23" s="45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K23" s="52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L23" s="52"/>
       <c r="M23" s="52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N23" s="52"/>
       <c r="O23" s="52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P23" s="52"/>
     </row>
@@ -2385,28 +2462,28 @@
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B25" s="40"/>
       <c r="C25" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="E25" s="40"/>
+        <v>66</v>
+      </c>
+      <c r="D25" s="104"/>
+      <c r="E25" s="40" t="s">
+        <v>98</v>
+      </c>
       <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
+      <c r="G25" s="104"/>
       <c r="H25" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I25" s="42"/>
       <c r="J25" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K25" s="34"/>
       <c r="L25" s="40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M25" s="40"/>
       <c r="N25" s="40"/>
@@ -2415,48 +2492,48 @@
     </row>
     <row r="26" spans="1:18">
       <c r="A26" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="54" t="s">
-        <v>66</v>
-      </c>
       <c r="C26" s="53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D26" s="53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E26" s="53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F26" s="53"/>
       <c r="G26" s="53"/>
       <c r="H26" s="53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I26" s="53"/>
       <c r="J26" s="53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K26" s="53"/>
       <c r="L26" s="40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M26" s="40"/>
       <c r="N26" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="O26" s="40" t="s">
         <v>97</v>
-      </c>
-      <c r="O26" s="40" t="s">
-        <v>98</v>
       </c>
       <c r="P26" s="48"/>
     </row>
     <row r="27" spans="1:18">
       <c r="A27" s="40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27" s="54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C27" s="24"/>
       <c r="D27" s="24"/>
@@ -2465,18 +2542,18 @@
       <c r="G27" s="24"/>
       <c r="H27" s="24"/>
       <c r="I27" s="24"/>
-      <c r="J27" s="94" t="s">
-        <v>142</v>
-      </c>
-      <c r="K27" s="94"/>
+      <c r="J27" s="93" t="s">
+        <v>141</v>
+      </c>
+      <c r="K27" s="93"/>
       <c r="L27" s="53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M27" s="53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N27" s="53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O27" s="53"/>
       <c r="P27" s="24"/>
@@ -2484,7 +2561,7 @@
     <row r="28" spans="1:18" ht="6" customHeight="1"/>
     <row r="29" spans="1:18" ht="15.75">
       <c r="A29" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" s="23"/>
       <c r="C29" s="23"/>
@@ -2504,131 +2581,125 @@
     </row>
     <row r="30" spans="1:18" ht="5.25" customHeight="1"/>
     <row r="31" spans="1:18" ht="14.25">
-      <c r="A31" s="83" t="s">
-        <v>69</v>
+      <c r="A31" s="81" t="s">
+        <v>68</v>
       </c>
       <c r="B31" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="E31" s="40" t="s">
-        <v>135</v>
-      </c>
-      <c r="F31" s="40"/>
+      <c r="F31" s="40" t="s">
+        <v>134</v>
+      </c>
       <c r="G31" s="40"/>
-      <c r="I31" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="J31" s="34"/>
+      <c r="H31" s="40"/>
       <c r="K31" s="34" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="L31" s="34"/>
       <c r="M31" s="34" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N31" s="34"/>
-      <c r="O31" s="98" t="s">
-        <v>38</v>
-      </c>
-      <c r="P31" s="98"/>
+      <c r="O31" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="P31" s="34"/>
     </row>
     <row r="32" spans="1:18">
-      <c r="A32" s="84" t="s">
-        <v>49</v>
+      <c r="A32" s="82" t="s">
+        <v>48</v>
       </c>
       <c r="B32" s="55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C32" s="55" t="s">
-        <v>73</v>
-      </c>
-      <c r="D32" s="86" t="s">
-        <v>137</v>
-      </c>
-      <c r="E32" s="96" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" s="84" t="s">
+        <v>136</v>
+      </c>
+      <c r="F32" s="95" t="s">
+        <v>144</v>
+      </c>
+      <c r="G32" s="34"/>
+      <c r="H32" s="96" t="s">
         <v>145</v>
       </c>
-      <c r="F32" s="34"/>
-      <c r="G32" s="97" t="s">
-        <v>146</v>
-      </c>
-      <c r="I32" s="54" t="s">
-        <v>66</v>
-      </c>
-      <c r="J32" s="49"/>
       <c r="K32" s="54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L32" s="49"/>
       <c r="M32" s="54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N32" s="49"/>
-      <c r="O32" s="99" t="s">
-        <v>73</v>
-      </c>
-      <c r="P32" s="99"/>
+      <c r="O32" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="P32" s="49"/>
     </row>
     <row r="33" spans="1:18" ht="14.25" customHeight="1">
-      <c r="A33" s="84" t="s">
-        <v>50</v>
+      <c r="A33" s="82" t="s">
+        <v>49</v>
       </c>
       <c r="B33" s="55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C33" s="55" t="s">
-        <v>73</v>
-      </c>
-      <c r="D33" s="86" t="s">
-        <v>138</v>
-      </c>
-      <c r="E33" s="49"/>
-      <c r="F33" s="49" t="s">
-        <v>71</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="D33" s="84" t="s">
+        <v>137</v>
+      </c>
+      <c r="F33" s="49"/>
       <c r="G33" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="I33" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="J33" s="34"/>
+        <v>70</v>
+      </c>
+      <c r="H33" s="49" t="s">
+        <v>72</v>
+      </c>
       <c r="K33" s="34" t="s">
         <v>102</v>
       </c>
       <c r="L33" s="34"/>
-      <c r="O33" s="100"/>
-      <c r="P33" s="100"/>
+      <c r="M33" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="N33" s="34"/>
+      <c r="O33" s="97" t="s">
+        <v>148</v>
+      </c>
+      <c r="P33" s="97"/>
     </row>
     <row r="34" spans="1:18">
-      <c r="A34" s="85" t="s">
-        <v>136</v>
+      <c r="A34" s="83" t="s">
+        <v>135</v>
       </c>
       <c r="B34" s="56" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C34" s="56" t="s">
-        <v>73</v>
-      </c>
-      <c r="D34" s="86" t="s">
-        <v>139</v>
+        <v>72</v>
+      </c>
+      <c r="D34" s="108" t="s">
+        <v>138</v>
       </c>
       <c r="E34" s="25"/>
-      <c r="I34" s="54" t="s">
-        <v>66</v>
-      </c>
-      <c r="J34" s="49"/>
       <c r="K34" s="54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L34" s="49"/>
-      <c r="M34" s="57"/>
-      <c r="N34" s="57"/>
-      <c r="O34" s="100"/>
-      <c r="P34" s="100"/>
+      <c r="M34" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="N34" s="49"/>
+      <c r="O34" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="P34" s="98"/>
     </row>
     <row r="35" spans="1:18" ht="6" customHeight="1">
       <c r="A35" s="25"/>
@@ -2636,7 +2707,7 @@
     </row>
     <row r="36" spans="1:18" ht="15.75">
       <c r="A36" s="26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B36" s="23"/>
       <c r="C36" s="23"/>
@@ -2656,27 +2727,27 @@
     </row>
     <row r="37" spans="1:18" ht="5.25" customHeight="1"/>
     <row r="38" spans="1:18" s="38" customFormat="1">
-      <c r="A38" s="58" t="s">
-        <v>106</v>
+      <c r="A38" s="57" t="s">
+        <v>105</v>
       </c>
       <c r="B38" s="34"/>
       <c r="C38" s="25"/>
       <c r="D38" s="34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E38" s="25"/>
       <c r="F38" s="25"/>
       <c r="G38" s="34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H38" s="25"/>
       <c r="I38" s="34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J38" s="34"/>
       <c r="K38" s="25"/>
       <c r="L38" s="34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M38" s="34"/>
       <c r="N38" s="34"/>
@@ -2691,109 +2762,109 @@
       </c>
       <c r="B39" s="49"/>
       <c r="C39" s="49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D39" s="49">
         <v>10</v>
       </c>
       <c r="E39" s="49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F39" s="49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G39" s="49"/>
       <c r="H39" s="49"/>
       <c r="I39" s="49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J39" s="49"/>
       <c r="L39" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M39" s="34"/>
       <c r="N39" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O39" s="34"/>
     </row>
     <row r="40" spans="1:18">
-      <c r="A40" s="87" t="s">
-        <v>50</v>
-      </c>
-      <c r="B40" s="88" t="s">
-        <v>131</v>
+      <c r="A40" s="85" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="86" t="s">
+        <v>130</v>
       </c>
       <c r="C40" s="36" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D40" s="36"/>
       <c r="E40" s="36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F40" s="37"/>
       <c r="H40" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I40" s="34"/>
       <c r="K40" s="40"/>
-      <c r="L40" s="61"/>
-      <c r="M40" s="61"/>
-      <c r="N40" s="61"/>
-      <c r="O40" s="61"/>
+      <c r="L40" s="60"/>
+      <c r="M40" s="60"/>
+      <c r="N40" s="60"/>
+      <c r="O40" s="60"/>
       <c r="P40" s="40"/>
     </row>
     <row r="41" spans="1:18" ht="14.25">
-      <c r="A41" s="89" t="s">
-        <v>61</v>
-      </c>
-      <c r="B41" s="101">
+      <c r="A41" s="87" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="99">
         <v>23</v>
       </c>
       <c r="C41" s="55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D41" s="55"/>
       <c r="E41" s="55" t="s">
-        <v>73</v>
-      </c>
-      <c r="F41" s="59"/>
+        <v>72</v>
+      </c>
+      <c r="F41" s="58"/>
       <c r="H41" s="49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I41" s="49"/>
       <c r="K41" s="40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L41" s="40"/>
       <c r="M41" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="N41" s="40" t="s">
         <v>97</v>
-      </c>
-      <c r="N41" s="40" t="s">
-        <v>98</v>
       </c>
       <c r="O41" s="48"/>
       <c r="P41" s="40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="14.25">
-      <c r="A42" s="90" t="s">
-        <v>62</v>
-      </c>
-      <c r="B42" s="101">
+      <c r="A42" s="88" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" s="99">
         <v>-3</v>
       </c>
       <c r="C42" s="56" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D42" s="56"/>
       <c r="E42" s="56" t="s">
-        <v>73</v>
-      </c>
-      <c r="F42" s="60"/>
+        <v>72</v>
+      </c>
+      <c r="F42" s="59"/>
       <c r="K42" s="53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L42" s="53"/>
       <c r="M42" s="53"/>
@@ -2804,7 +2875,7 @@
     <row r="43" spans="1:18" ht="6" customHeight="1"/>
     <row r="44" spans="1:18" ht="15.75">
       <c r="A44" s="26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B44" s="23"/>
       <c r="C44" s="23"/>
@@ -2825,35 +2896,35 @@
     <row r="45" spans="1:18" ht="5.25" customHeight="1"/>
     <row r="46" spans="1:18">
       <c r="A46" s="34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B46" s="34"/>
       <c r="C46" s="34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D46" s="34"/>
       <c r="E46" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F46" s="34"/>
       <c r="G46" s="34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H46" s="34"/>
       <c r="I46" s="34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J46" s="34"/>
       <c r="K46" s="34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L46" s="34"/>
       <c r="M46" s="34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N46" s="34"/>
       <c r="O46" s="34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P46" s="34"/>
     </row>
@@ -2863,65 +2934,65 @@
       </c>
       <c r="B47" s="31"/>
       <c r="C47" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D47" s="31"/>
       <c r="E47" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F47" s="31"/>
       <c r="G47" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H47" s="31"/>
       <c r="I47" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J47" s="31"/>
       <c r="K47" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L47" s="31"/>
       <c r="M47" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N47" s="31"/>
       <c r="O47" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P47" s="31"/>
     </row>
     <row r="48" spans="1:18">
-      <c r="B48" s="80" t="s">
-        <v>131</v>
-      </c>
-      <c r="C48" s="94">
+      <c r="B48" s="78" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" s="93">
         <v>323125</v>
       </c>
-      <c r="D48" s="94"/>
-      <c r="E48" s="94">
+      <c r="D48" s="93"/>
+      <c r="E48" s="93">
         <v>26.5</v>
       </c>
-      <c r="F48" s="94"/>
-      <c r="G48" s="91" t="s">
-        <v>73</v>
-      </c>
-      <c r="H48" s="91"/>
-      <c r="I48" s="91" t="s">
-        <v>73</v>
-      </c>
-      <c r="J48" s="91"/>
-      <c r="K48" s="102">
+      <c r="F48" s="93"/>
+      <c r="G48" s="89" t="s">
+        <v>72</v>
+      </c>
+      <c r="H48" s="89"/>
+      <c r="I48" s="89" t="s">
+        <v>72</v>
+      </c>
+      <c r="J48" s="89"/>
+      <c r="K48" s="100">
         <v>43061.993819444448</v>
       </c>
-      <c r="L48" s="94"/>
+      <c r="L48" s="93"/>
     </row>
     <row r="49" spans="1:16" ht="5.25" customHeight="1">
       <c r="K49" s="25"/>
     </row>
     <row r="50" spans="1:16" ht="15.75">
       <c r="A50" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B50" s="23"/>
       <c r="C50" s="23"/>
@@ -2941,8 +3012,18 @@
     </row>
     <row r="51" spans="1:16" ht="5.25" customHeight="1"/>
     <row r="52" spans="1:16">
-      <c r="A52" s="103" t="s">
+      <c r="A52" s="101" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
+      <c r="A54" s="25" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="102" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2988,18 +3069,18 @@
   <sheetData>
     <row r="1" spans="1:11" ht="24.75" customHeight="1"/>
     <row r="2" spans="1:11" ht="60.4" customHeight="1">
-      <c r="C2" s="71" t="s">
+      <c r="C2" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="72" t="s">
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="70" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="18" customHeight="1">
-      <c r="G3" s="72"/>
+      <c r="G3" s="70"/>
     </row>
     <row r="4" spans="1:11" ht="18" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -3011,7 +3092,7 @@
       <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="72"/>
+      <c r="G4" s="70"/>
     </row>
     <row r="5" spans="1:11" ht="18.95" customHeight="1">
       <c r="A5" s="4" t="s">
@@ -3020,7 +3101,7 @@
       <c r="C5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="72"/>
+      <c r="G5" s="70"/>
     </row>
     <row r="6" spans="1:11" ht="18.95" customHeight="1">
       <c r="A6" s="4" t="s">
@@ -3029,7 +3110,7 @@
       <c r="C6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="72"/>
+      <c r="G6" s="70"/>
     </row>
     <row r="7" spans="1:11" ht="18.95" customHeight="1">
       <c r="A7" s="4" t="s">
@@ -3038,19 +3119,19 @@
       <c r="C7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="72"/>
+      <c r="G7" s="70"/>
     </row>
     <row r="10" spans="1:11" ht="22.9" customHeight="1">
-      <c r="A10" s="73" t="s">
+      <c r="A10" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="71"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="4" t="s">
@@ -3076,8 +3157,8 @@
         <v>11</v>
       </c>
       <c r="F13" s="8"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="74"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="72"/>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="4" t="s">
@@ -3087,8 +3168,8 @@
         <v>12</v>
       </c>
       <c r="F14" s="8"/>
-      <c r="G14" s="74"/>
-      <c r="H14" s="74"/>
+      <c r="G14" s="72"/>
+      <c r="H14" s="72"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="4" t="s">
@@ -3098,8 +3179,8 @@
         <v>13</v>
       </c>
       <c r="F15" s="8"/>
-      <c r="G15" s="74"/>
-      <c r="H15" s="74"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="72"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="4"/>
@@ -3111,16 +3192,16 @@
       <c r="A17" s="4"/>
     </row>
     <row r="18" spans="1:11" ht="22.9" customHeight="1">
-      <c r="A18" s="73" t="s">
+      <c r="A18" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="73"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
-      <c r="H18" s="73"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="71"/>
     </row>
     <row r="20" spans="1:11" ht="21.4" customHeight="1">
       <c r="A20" s="10" t="s">
@@ -3156,84 +3237,84 @@
         <v>16</v>
       </c>
       <c r="B22" s="11"/>
-      <c r="C22" s="75" t="s">
+      <c r="C22" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="75"/>
-      <c r="E22" s="75"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="75"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73"/>
     </row>
     <row r="23" spans="1:11" ht="55.35" customHeight="1">
       <c r="A23" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B23" s="11"/>
-      <c r="C23" s="76"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="76"/>
-      <c r="G23" s="76"/>
-      <c r="H23" s="76"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="74"/>
     </row>
     <row r="25" spans="1:11" ht="19.899999999999999" customHeight="1">
-      <c r="A25" s="77" t="s">
+      <c r="A25" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="77"/>
-      <c r="C25" s="78"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="76"/>
       <c r="D25" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="79" t="s">
+      <c r="E25" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="79"/>
-      <c r="G25" s="79"/>
-      <c r="H25" s="79"/>
+      <c r="F25" s="77"/>
+      <c r="G25" s="77"/>
+      <c r="H25" s="77"/>
     </row>
     <row r="26" spans="1:11" ht="15.95" customHeight="1">
-      <c r="A26" s="67" t="s">
+      <c r="A26" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="68"/>
-      <c r="C26" s="69"/>
+      <c r="B26" s="66"/>
+      <c r="C26" s="67"/>
       <c r="D26" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="70"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="70"/>
-      <c r="H26" s="70"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="67" t="s">
+      <c r="A27" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="68"/>
-      <c r="C27" s="69"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="67"/>
       <c r="D27" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="70"/>
-      <c r="F27" s="70"/>
-      <c r="G27" s="70"/>
-      <c r="H27" s="70"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="67" t="s">
+      <c r="A28" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="68"/>
-      <c r="C28" s="69"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="67"/>
       <c r="D28" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="70"/>
-      <c r="F28" s="70"/>
-      <c r="G28" s="70"/>
-      <c r="H28" s="70"/>
+      <c r="E28" s="68"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="68"/>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="19"/>

</xml_diff>

<commit_message>
staircase/specific protocol/ instructions particulieres
</commit_message>
<xml_diff>
--- a/lib/PHPExcel/templates/FT.xlsx
+++ b/lib/PHPExcel/templates/FT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -22,41 +22,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="118">
-  <si>
-    <t>2017-11-21</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="100">
   <si>
     <t>Drawing</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF44546A"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Strain Contrôle Fatigue Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFA5A5A5"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Ce document fait office de fiche technique.</t>
-    </r>
-  </si>
-  <si>
     <t>Job</t>
   </si>
   <si>
@@ -69,18 +39,6 @@
     <t>FT - 48558</t>
   </si>
   <si>
-    <t>8000-00000-1</t>
-  </si>
-  <si>
-    <t>Dummy</t>
-  </si>
-  <si>
-    <t>PGO</t>
-  </si>
-  <si>
-    <t>PQF</t>
-  </si>
-  <si>
     <t>Frame Informations</t>
   </si>
   <si>
@@ -162,15 +120,9 @@
     <t>/</t>
   </si>
   <si>
-    <t>Fréquence (Hz)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Opérateur</t>
-  </si>
-  <si>
     <t>STL REALISE</t>
   </si>
   <si>
@@ -264,9 +216,6 @@
     <t>UnderPeak</t>
   </si>
   <si>
-    <t>STL requierement</t>
-  </si>
-  <si>
     <t>After STL</t>
   </si>
   <si>
@@ -291,36 +240,9 @@
     <t>Switch to Load</t>
   </si>
   <si>
-    <t>M12-1-P-35-55</t>
-  </si>
-  <si>
-    <t>M12-1-P-35-56</t>
-  </si>
-  <si>
-    <t>TZ1000-Tz10001-TZ10002</t>
-  </si>
-  <si>
-    <t>xxx</t>
-  </si>
-  <si>
-    <t>xxxxx</t>
-  </si>
-  <si>
-    <t>485-920-525-0</t>
-  </si>
-  <si>
-    <t>INCO718PQW</t>
-  </si>
-  <si>
-    <t>Diameters</t>
-  </si>
-  <si>
     <t>Raw Data</t>
   </si>
   <si>
-    <t>SNECMA</t>
-  </si>
-  <si>
     <t>Sens.</t>
   </si>
   <si>
@@ -358,18 +280,6 @@
   </si>
   <si>
     <t>Dilatation</t>
-  </si>
-  <si>
-    <t>(-0.216 %)</t>
-  </si>
-  <si>
-    <t>True Sine</t>
-  </si>
-  <si>
-    <t>---Quels commentaires afficher ? Instruction/commentaire job, split, eprouvettes ?</t>
-  </si>
-  <si>
-    <t>affichage delai ?</t>
   </si>
   <si>
     <t>Grey cell : unused equipement or information (unless specified) -- Instructions on GPM need to be checked if checker is empty</t>
@@ -464,30 +374,6 @@
   </si>
   <si>
     <r>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color rgb="FF8497B0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF8497B0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> cycle</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <sz val="10"/>
         <color rgb="FF8497B0"/>
@@ -530,30 +416,6 @@
   </si>
   <si>
     <r>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color rgb="FF8497B0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF8497B0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Check</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Rupture-</t>
     </r>
     <r>
@@ -566,6 +428,90 @@
       <t>ERT(kN)</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>st</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> cycle</t>
+    </r>
+  </si>
+  <si>
+    <t>Fréquency (Hz)</t>
+  </si>
+  <si>
+    <t>STL requirement</t>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>st</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Check</t>
+    </r>
+  </si>
+  <si>
+    <t>Dimension 1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF44546A"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Strain Contrôle Fatigue Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFA5A5A5"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>This document acts as technical sheet.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -591,11 +537,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FFC00000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
@@ -757,6 +698,12 @@
       <color rgb="FF203764"/>
       <name val="Wingdings"/>
       <charset val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -928,197 +875,197 @@
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="22" fontId="26" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="22" fontId="27" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -1188,11 +1135,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>66062</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="447675" cy="1938130"/>
+    <xdr:ext cx="381811" cy="1938130"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="4" name="Image 3">
@@ -1207,15 +1154,21 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6708913" y="1"/>
-          <a:ext cx="447675" cy="1938130"/>
+          <a:off x="6774975" y="0"/>
+          <a:ext cx="381811" cy="1938130"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1517,7 +1470,7 @@
   <dimension ref="A1:R68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="O2" sqref="O2:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
@@ -1530,7 +1483,7 @@
     <row r="1" spans="1:18" ht="24.75" hidden="1" customHeight="1"/>
     <row r="2" spans="1:18" ht="60.4" customHeight="1">
       <c r="C2" s="4" t="s">
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -1544,7 +1497,7 @@
       <c r="M2" s="4"/>
       <c r="N2" s="3"/>
       <c r="O2" s="78" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="18" customHeight="1">
@@ -1552,116 +1505,96 @@
     </row>
     <row r="4" spans="1:18" ht="18" customHeight="1">
       <c r="A4" s="18" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="19"/>
       <c r="D4" s="18" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="19"/>
       <c r="G4" s="18" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H4" s="18"/>
       <c r="I4" s="21"/>
       <c r="J4" s="18" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="K4" s="18"/>
       <c r="L4" s="21"/>
       <c r="M4" s="18"/>
       <c r="N4" s="22" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="O4" s="78"/>
     </row>
     <row r="5" spans="1:18" ht="18.95" customHeight="1">
-      <c r="A5" s="55" t="s">
-        <v>7</v>
-      </c>
+      <c r="A5" s="55"/>
       <c r="B5" s="55"/>
       <c r="C5" s="76"/>
-      <c r="D5" s="55" t="s">
-        <v>8</v>
-      </c>
+      <c r="D5" s="55"/>
       <c r="E5" s="55"/>
       <c r="F5" s="76"/>
-      <c r="G5" s="55">
-        <v>1</v>
-      </c>
+      <c r="G5" s="55"/>
       <c r="H5" s="55"/>
       <c r="I5" s="77"/>
-      <c r="J5" s="55">
-        <v>48558</v>
-      </c>
+      <c r="J5" s="55"/>
       <c r="K5" s="55"/>
       <c r="L5" s="77"/>
-      <c r="M5" s="55">
-        <v>5</v>
-      </c>
+      <c r="M5" s="55"/>
       <c r="N5" s="55"/>
       <c r="O5" s="78"/>
     </row>
     <row r="6" spans="1:18" ht="18.95" customHeight="1">
       <c r="A6" s="18" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="19"/>
       <c r="D6" s="18" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="19"/>
       <c r="G6" s="18" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H6" s="20"/>
       <c r="I6" s="23"/>
       <c r="J6" s="18" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="K6" s="20"/>
       <c r="L6" s="24"/>
       <c r="M6" s="20"/>
       <c r="N6" s="25" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="O6" s="78"/>
     </row>
     <row r="7" spans="1:18" ht="18.95" customHeight="1">
-      <c r="A7" s="55">
-        <v>20025</v>
-      </c>
+      <c r="A7" s="55"/>
       <c r="B7" s="55"/>
       <c r="C7" s="76"/>
-      <c r="D7" s="55" t="s">
-        <v>90</v>
-      </c>
+      <c r="D7" s="55"/>
       <c r="E7" s="55"/>
       <c r="F7" s="76"/>
-      <c r="G7" s="55" t="s">
-        <v>9</v>
-      </c>
+      <c r="G7" s="55"/>
       <c r="H7" s="55"/>
       <c r="I7" s="77"/>
-      <c r="J7" s="55" t="s">
-        <v>10</v>
-      </c>
+      <c r="J7" s="55"/>
       <c r="K7" s="55"/>
       <c r="L7" s="77"/>
-      <c r="M7" s="55" t="s">
-        <v>0</v>
-      </c>
+      <c r="M7" s="55"/>
       <c r="N7" s="55"/>
       <c r="O7" s="78"/>
     </row>
     <row r="8" spans="1:18" ht="6" customHeight="1"/>
     <row r="9" spans="1:18" ht="15" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
@@ -1682,176 +1615,122 @@
     <row r="10" spans="1:18" ht="5.25" customHeight="1"/>
     <row r="11" spans="1:18" s="8" customFormat="1">
       <c r="A11" s="20" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="20" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="20" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="26"/>
       <c r="J11" s="27" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="K11" s="27" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="L11" s="27" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="M11" s="27" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="N11" s="27" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="O11" s="27" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="P11" s="28" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
     </row>
     <row r="12" spans="1:18" ht="14.25">
-      <c r="A12" s="55" t="s">
-        <v>81</v>
-      </c>
+      <c r="A12" s="55"/>
       <c r="B12" s="55"/>
-      <c r="C12" s="55" t="s">
-        <v>82</v>
-      </c>
+      <c r="C12" s="55"/>
       <c r="D12" s="55"/>
-      <c r="E12" s="55">
-        <v>60001</v>
-      </c>
+      <c r="E12" s="55"/>
       <c r="F12" s="55"/>
       <c r="G12" s="66" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H12" s="55"/>
       <c r="I12" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="K12" s="72">
-        <v>80</v>
-      </c>
-      <c r="L12" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="M12" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="N12" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="O12" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="P12" s="73" t="s">
-        <v>39</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="J12" s="72"/>
+      <c r="K12" s="72"/>
+      <c r="L12" s="72"/>
+      <c r="M12" s="72"/>
+      <c r="N12" s="72"/>
+      <c r="O12" s="72"/>
+      <c r="P12" s="73"/>
     </row>
     <row r="13" spans="1:18" s="8" customFormat="1">
       <c r="A13" s="20" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B13" s="20"/>
       <c r="C13" s="20" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="20" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
       <c r="I13" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="72" t="s">
-        <v>85</v>
-      </c>
-      <c r="K13" s="72">
-        <v>100</v>
-      </c>
-      <c r="L13" s="72">
-        <v>3</v>
-      </c>
-      <c r="M13" s="72">
-        <v>0.3</v>
-      </c>
-      <c r="N13" s="72">
-        <v>0</v>
-      </c>
-      <c r="O13" s="72">
-        <v>10</v>
-      </c>
-      <c r="P13" s="73">
-        <v>1</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="J13" s="72"/>
+      <c r="K13" s="72"/>
+      <c r="L13" s="72"/>
+      <c r="M13" s="72"/>
+      <c r="N13" s="72"/>
+      <c r="O13" s="72"/>
+      <c r="P13" s="73"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
     </row>
     <row r="14" spans="1:18" ht="14.25">
-      <c r="A14" s="55">
-        <v>50001</v>
-      </c>
+      <c r="A14" s="55"/>
       <c r="B14" s="55"/>
-      <c r="C14" s="55">
-        <v>40001</v>
-      </c>
+      <c r="C14" s="55"/>
       <c r="D14" s="55"/>
-      <c r="E14" s="55" t="s">
-        <v>83</v>
-      </c>
+      <c r="E14" s="55"/>
       <c r="F14" s="55"/>
       <c r="G14" s="55"/>
       <c r="H14" s="55"/>
       <c r="I14" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="74">
-        <v>10005</v>
-      </c>
-      <c r="K14" s="74">
-        <v>5</v>
-      </c>
-      <c r="L14" s="74">
-        <v>1500</v>
-      </c>
-      <c r="M14" s="74">
-        <v>150</v>
-      </c>
-      <c r="N14" s="74">
-        <v>0</v>
-      </c>
-      <c r="O14" s="74">
-        <v>40</v>
-      </c>
-      <c r="P14" s="75">
-        <v>0.5</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="J14" s="74"/>
+      <c r="K14" s="74"/>
+      <c r="L14" s="74"/>
+      <c r="M14" s="74"/>
+      <c r="N14" s="74"/>
+      <c r="O14" s="74"/>
+      <c r="P14" s="75"/>
     </row>
     <row r="15" spans="1:18" ht="6" customHeight="1">
       <c r="A15" s="2"/>
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1">
       <c r="A16" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
@@ -1881,7 +1760,7 @@
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
       <c r="E18" s="20" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
@@ -1889,7 +1768,7 @@
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
       <c r="K18" s="20" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="L18" s="20"/>
       <c r="M18" s="20"/>
@@ -1899,105 +1778,89 @@
     </row>
     <row r="19" spans="1:18" s="8" customFormat="1">
       <c r="A19" s="20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="20" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="20" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="F19" s="20"/>
       <c r="G19" s="20" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H19" s="20"/>
       <c r="I19" s="20" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J19" s="20"/>
       <c r="K19" s="20" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="L19" s="20"/>
       <c r="M19" s="20" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="N19" s="20"/>
       <c r="O19" s="20" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="P19" s="20"/>
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
     </row>
     <row r="20" spans="1:18">
-      <c r="A20" s="55" t="s">
-        <v>86</v>
-      </c>
+      <c r="A20" s="55"/>
       <c r="B20" s="55"/>
-      <c r="C20" s="55" t="s">
-        <v>87</v>
-      </c>
+      <c r="C20" s="55"/>
       <c r="D20" s="55"/>
-      <c r="E20" s="70">
-        <v>4.37</v>
-      </c>
+      <c r="E20" s="70"/>
       <c r="F20" s="55"/>
-      <c r="G20" s="55" t="s">
-        <v>39</v>
-      </c>
+      <c r="G20" s="55"/>
       <c r="H20" s="55"/>
-      <c r="I20" s="55" t="s">
-        <v>39</v>
-      </c>
+      <c r="I20" s="55"/>
       <c r="J20" s="55"/>
-      <c r="K20" s="55">
-        <v>350</v>
-      </c>
+      <c r="K20" s="55"/>
       <c r="L20" s="55"/>
-      <c r="M20" s="55">
-        <v>350.8</v>
-      </c>
+      <c r="M20" s="55"/>
       <c r="N20" s="55"/>
-      <c r="O20" s="55">
-        <v>2000000</v>
-      </c>
+      <c r="O20" s="55"/>
       <c r="P20" s="55"/>
     </row>
     <row r="21" spans="1:18" s="8" customFormat="1">
       <c r="A21" s="20"/>
       <c r="B21" s="32" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="20" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="F21" s="20"/>
       <c r="G21" s="20" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H21" s="20"/>
       <c r="I21" s="33"/>
       <c r="J21" s="34" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="K21" s="20" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="L21" s="20"/>
       <c r="M21" s="20" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="N21" s="20"/>
       <c r="O21" s="20" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="P21" s="20"/>
       <c r="Q21" s="6"/>
@@ -2005,73 +1868,57 @@
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="B22" s="57">
-        <v>180</v>
-      </c>
-      <c r="C22" s="55" t="s">
-        <v>39</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="B22" s="57"/>
+      <c r="C22" s="55"/>
       <c r="D22" s="55"/>
-      <c r="E22" s="55">
-        <v>1</v>
-      </c>
+      <c r="E22" s="55"/>
       <c r="F22" s="55"/>
-      <c r="G22" s="55" t="s">
-        <v>105</v>
-      </c>
+      <c r="G22" s="55"/>
       <c r="H22" s="55"/>
       <c r="I22" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="J22" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="K22" s="55">
-        <v>0.6</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="K22" s="55"/>
       <c r="L22" s="55"/>
-      <c r="M22" s="55">
-        <v>0.06</v>
-      </c>
+      <c r="M22" s="55"/>
       <c r="N22" s="55"/>
-      <c r="O22" s="55">
-        <v>12</v>
-      </c>
+      <c r="O22" s="55"/>
       <c r="P22" s="55"/>
     </row>
     <row r="23" spans="1:18" ht="15.75">
       <c r="A23" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="B23" s="71">
-        <v>170</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="B23" s="71"/>
       <c r="C23" s="69" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D23" s="69"/>
       <c r="E23" s="16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F23" s="16"/>
       <c r="G23" s="17"/>
       <c r="H23" s="16"/>
       <c r="I23" s="17"/>
       <c r="J23" s="41" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="K23" s="69" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="L23" s="69"/>
       <c r="M23" s="69" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="N23" s="69"/>
       <c r="O23" s="69" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="P23" s="69"/>
     </row>
@@ -2095,28 +1942,28 @@
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="37" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B25" s="37"/>
       <c r="C25" s="37" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D25" s="38"/>
       <c r="E25" s="37" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F25" s="37"/>
       <c r="G25" s="38"/>
       <c r="H25" s="39" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="I25" s="39"/>
       <c r="J25" s="20" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="K25" s="20"/>
       <c r="L25" s="37" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="M25" s="37"/>
       <c r="N25" s="37"/>
@@ -2125,48 +1972,48 @@
     </row>
     <row r="26" spans="1:18">
       <c r="A26" s="37" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B26" s="66" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C26" s="64" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D26" s="64" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E26" s="64" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F26" s="64"/>
       <c r="G26" s="64"/>
       <c r="H26" s="64" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="I26" s="64"/>
       <c r="J26" s="64" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="K26" s="64"/>
       <c r="L26" s="37" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="M26" s="37"/>
       <c r="N26" s="40" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="O26" s="37" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="P26" s="37"/>
     </row>
     <row r="27" spans="1:18">
       <c r="A27" s="37" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B27" s="66" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C27" s="68"/>
       <c r="D27" s="68"/>
@@ -2175,18 +2022,16 @@
       <c r="G27" s="68"/>
       <c r="H27" s="68"/>
       <c r="I27" s="68"/>
-      <c r="J27" s="11" t="s">
-        <v>104</v>
-      </c>
+      <c r="J27" s="11"/>
       <c r="K27" s="11"/>
       <c r="L27" s="64" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="M27" s="64" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="N27" s="64" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="O27" s="64"/>
       <c r="P27" s="68"/>
@@ -2194,7 +2039,7 @@
     <row r="28" spans="1:18" ht="6" customHeight="1"/>
     <row r="29" spans="1:18" ht="15.75">
       <c r="A29" s="14" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -2222,124 +2067,124 @@
     </row>
     <row r="31" spans="1:18" ht="14.25">
       <c r="A31" s="42" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F31" s="37" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="G31" s="37"/>
       <c r="H31" s="37"/>
       <c r="I31" s="19"/>
       <c r="K31" s="20" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="L31" s="20"/>
       <c r="M31" s="20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="N31" s="20"/>
       <c r="O31" s="20" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="P31" s="20"/>
     </row>
     <row r="32" spans="1:18">
       <c r="A32" s="43" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B32" s="60" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C32" s="60" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D32" s="45" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="F32" s="47" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="G32" s="20"/>
       <c r="H32" s="48" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="I32" s="19"/>
       <c r="K32" s="66" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L32" s="55"/>
       <c r="M32" s="66" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="N32" s="55"/>
       <c r="O32" s="66" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="P32" s="55"/>
     </row>
     <row r="33" spans="1:18" ht="14.25" customHeight="1">
       <c r="A33" s="43" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B33" s="60" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C33" s="60" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D33" s="45" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="F33" s="55"/>
       <c r="G33" s="55" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H33" s="55" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="K33" s="20" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="L33" s="20"/>
       <c r="M33" s="20" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="N33" s="20"/>
       <c r="O33" s="49" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="P33" s="49"/>
     </row>
     <row r="34" spans="1:18">
       <c r="A34" s="44" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="B34" s="62" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C34" s="62" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D34" s="46" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="E34" s="6"/>
       <c r="K34" s="66" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L34" s="55"/>
       <c r="M34" s="66" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="N34" s="55"/>
       <c r="O34" s="66" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="P34" s="67"/>
     </row>
@@ -2349,7 +2194,7 @@
     </row>
     <row r="36" spans="1:18" ht="15.75">
       <c r="A36" s="14" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -2370,26 +2215,26 @@
     <row r="37" spans="1:18" ht="5.25" customHeight="1"/>
     <row r="38" spans="1:18" s="8" customFormat="1">
       <c r="A38" s="50" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="B38" s="20"/>
       <c r="C38" s="19"/>
       <c r="D38" s="20" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="E38" s="19"/>
       <c r="F38" s="19"/>
       <c r="G38" s="20" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="H38" s="19"/>
       <c r="I38" s="20" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J38" s="20"/>
       <c r="K38" s="19"/>
       <c r="L38" s="20" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="M38" s="20"/>
       <c r="N38" s="20"/>
@@ -2399,55 +2244,51 @@
       <c r="R38" s="6"/>
     </row>
     <row r="39" spans="1:18">
-      <c r="A39" s="55">
-        <v>85000</v>
-      </c>
+      <c r="A39" s="55"/>
       <c r="B39" s="55"/>
       <c r="C39" s="55" t="s">
-        <v>39</v>
-      </c>
-      <c r="D39" s="55">
-        <v>10</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D39" s="55"/>
       <c r="E39" s="55" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F39" s="55" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G39" s="55"/>
       <c r="H39" s="55"/>
       <c r="I39" s="55" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="J39" s="55"/>
       <c r="K39" s="58"/>
       <c r="L39" s="20" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="M39" s="20"/>
       <c r="N39" s="20" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="O39" s="20"/>
     </row>
     <row r="40" spans="1:18">
       <c r="A40" s="51" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B40" s="54" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D40" s="27"/>
       <c r="E40" s="27" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="F40" s="28"/>
       <c r="H40" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I40" s="20"/>
       <c r="K40" s="9"/>
@@ -2459,57 +2300,53 @@
     </row>
     <row r="41" spans="1:18" ht="14.25">
       <c r="A41" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="B41" s="59">
-        <v>23</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B41" s="59"/>
       <c r="C41" s="60" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D41" s="60"/>
       <c r="E41" s="60" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F41" s="61"/>
       <c r="H41" s="55" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="I41" s="55"/>
       <c r="K41" s="37" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="L41" s="37"/>
       <c r="M41" s="40" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="N41" s="37" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="O41" s="37"/>
       <c r="P41" s="9" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="14.25">
       <c r="A42" s="53" t="s">
-        <v>28</v>
-      </c>
-      <c r="B42" s="59">
-        <v>-3</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B42" s="59"/>
       <c r="C42" s="62" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D42" s="62"/>
       <c r="E42" s="62" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F42" s="63"/>
       <c r="H42" s="58"/>
       <c r="I42" s="58"/>
       <c r="K42" s="64" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="L42" s="64"/>
       <c r="M42" s="64"/>
@@ -2520,7 +2357,7 @@
     <row r="43" spans="1:18" ht="6" customHeight="1"/>
     <row r="44" spans="1:18" ht="15.75">
       <c r="A44" s="14" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
@@ -2541,35 +2378,35 @@
     <row r="45" spans="1:18" ht="5.25" customHeight="1"/>
     <row r="46" spans="1:18">
       <c r="A46" s="20" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B46" s="20"/>
       <c r="C46" s="20" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="20" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="F46" s="20"/>
       <c r="G46" s="20" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="H46" s="20"/>
       <c r="I46" s="20" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="J46" s="20"/>
       <c r="K46" s="20" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L46" s="20"/>
       <c r="M46" s="20" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="N46" s="20"/>
       <c r="O46" s="20" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="P46" s="20"/>
     </row>
@@ -2579,57 +2416,51 @@
       </c>
       <c r="B47" s="55"/>
       <c r="C47" s="55" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D47" s="55"/>
       <c r="E47" s="55" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F47" s="55"/>
       <c r="G47" s="55" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H47" s="55"/>
       <c r="I47" s="55" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="J47" s="55"/>
       <c r="K47" s="55" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="L47" s="55"/>
       <c r="M47" s="55" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="N47" s="55"/>
       <c r="O47" s="55" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="P47" s="55"/>
     </row>
     <row r="48" spans="1:18">
       <c r="B48" s="36" t="s">
-        <v>94</v>
-      </c>
-      <c r="C48" s="57">
-        <v>323125</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="C48" s="57"/>
       <c r="D48" s="57"/>
-      <c r="E48" s="57">
-        <v>26.5</v>
-      </c>
+      <c r="E48" s="57"/>
       <c r="F48" s="57"/>
       <c r="G48" s="10" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H48" s="10"/>
       <c r="I48" s="10" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="J48" s="10"/>
-      <c r="K48" s="56">
-        <v>43061.993819444448</v>
-      </c>
+      <c r="K48" s="56"/>
       <c r="L48" s="57"/>
       <c r="M48" s="58"/>
       <c r="N48" s="58"/>
@@ -2641,7 +2472,7 @@
     </row>
     <row r="50" spans="1:16" ht="15.75">
       <c r="A50" s="14" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B50" s="15"/>
       <c r="C50" s="15"/>
@@ -2661,18 +2492,14 @@
     </row>
     <row r="51" spans="1:16" ht="5.25" customHeight="1"/>
     <row r="52" spans="1:16">
-      <c r="A52" s="12" t="s">
-        <v>106</v>
-      </c>
+      <c r="A52" s="12"/>
     </row>
     <row r="54" spans="1:16">
-      <c r="A54" s="6" t="s">
-        <v>107</v>
-      </c>
+      <c r="A54" s="6"/>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="13" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>